<commit_message>
çoklu girdi satırları benzersiz yapıldı
</commit_message>
<xml_diff>
--- a/docs/coklu_girdi.xlsx
+++ b/docs/coklu_girdi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammed.bulut\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12973F89-1697-4C18-9A46-4262BB79D7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2FFBB7-3B4A-449C-AF58-AB15311EB96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>SIRA</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Fatma KARACA</t>
+  </si>
+  <si>
+    <t>Fatma KARA</t>
   </si>
 </sst>
 </file>
@@ -841,7 +844,7 @@
   <dimension ref="A1:AB137"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C3" sqref="A3:XFD3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -990,7 +993,7 @@
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="9"/>

</xml_diff>